<commit_message>
update: refresh Excel files with June 2025 data from VPS production
- Downloaded latest Excel files from VPS production server
- Updated all 6 Excel files: Bulk Actions, Cost Allocation, Vessel Classifications, Vessel Manifests, Voyage Events, Voyage List
- Files contain June 2025 operational data for enhanced analytics accuracy
- Monthly upload components added for future data management

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/excel-data/excel-files/Vessel Classifications.xlsx
+++ b/excel-data/excel-files/Vessel Classifications.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365-my.sharepoint.com/personal/neal_smothers_bp_com/Documents/PowerBI/PowerBI Data/Drill_Prod Dashboard/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nealasmothers/Downloads/logisticsdashboard/excel-data/excel-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="137" documentId="8_{C5642CE8-693A-4DDE-AB7A-1F5046830054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2239338B-96B1-8446-9B83-8C02277F039B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA026AD-5509-4F40-88EA-D403424E8C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{CBC69028-2E6F-46B8-97F1-40991527D390}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="49">
   <si>
     <t>Vessel Name</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>Charlie Comeaux</t>
+  </si>
+  <si>
+    <t>Thunder</t>
   </si>
 </sst>
 </file>
@@ -251,10 +254,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -577,7 +576,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -980,6 +979,20 @@
         <v>7</v>
       </c>
     </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>252</v>
+      </c>
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>38</v>

</xml_diff>